<commit_message>
add payload for updateEnrollment coordinate
</commit_message>
<xml_diff>
--- a/sample-format/programIndicatorsNameUpdate.xlsx
+++ b/sample-format/programIndicatorsNameUpdate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717134F4-5DD6-4B9F-BCB5-F3E47DEB644F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6028CA41-F8AE-4939-8FF8-8433F088E83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -39,16 +39,484 @@
     <t>uid</t>
   </si>
   <si>
-    <t>HcBcXMBr1hr</t>
-  </si>
-  <si>
-    <t>Escherichia coli isolated - Non-urine sample temp</t>
-  </si>
-  <si>
-    <t>Enterobacteriaceae - Total events</t>
-  </si>
-  <si>
-    <t>QSOBcLiy2vg</t>
+    <t>uUNjyz36E7x</t>
+  </si>
+  <si>
+    <t>UTCAbe6f7OP</t>
+  </si>
+  <si>
+    <t>kDHjLu9bKbW</t>
+  </si>
+  <si>
+    <t>wV5HXjJLpNJ</t>
+  </si>
+  <si>
+    <t>knPkKzNUwyh</t>
+  </si>
+  <si>
+    <t>iWsJVW7w6W5</t>
+  </si>
+  <si>
+    <t>dmwwFSMg4kN</t>
+  </si>
+  <si>
+    <t>rPdi3eVESWJ</t>
+  </si>
+  <si>
+    <t>APLotRP5FoT</t>
+  </si>
+  <si>
+    <t>JRUtgSfLARM</t>
+  </si>
+  <si>
+    <t>LxjEw7Tk2vW</t>
+  </si>
+  <si>
+    <t>gQRXLuuR1Pt</t>
+  </si>
+  <si>
+    <t>g0Y9ZI85LkQ</t>
+  </si>
+  <si>
+    <t>OzWwZVuOHng</t>
+  </si>
+  <si>
+    <t>GV7fXZNfeS3</t>
+  </si>
+  <si>
+    <t>rqcbyvd6YR5</t>
+  </si>
+  <si>
+    <t>gr5XSwlbLf2</t>
+  </si>
+  <si>
+    <t>BjRXtTGVRmN</t>
+  </si>
+  <si>
+    <t>JnGPuxkTXhj</t>
+  </si>
+  <si>
+    <t>hSEGIzZYyRX</t>
+  </si>
+  <si>
+    <t>LLVanXQNj1W</t>
+  </si>
+  <si>
+    <t>MfpFZlgorOh</t>
+  </si>
+  <si>
+    <t>Yvb6cCAxTSU</t>
+  </si>
+  <si>
+    <t>veEhc7m2XRL</t>
+  </si>
+  <si>
+    <t>a5cq6gSGYuz</t>
+  </si>
+  <si>
+    <t>QyQH1U9cq1A</t>
+  </si>
+  <si>
+    <t>qX1sOOoZ7nI</t>
+  </si>
+  <si>
+    <t>BqIsY3tvPw6</t>
+  </si>
+  <si>
+    <t>TKKXBACDmmP</t>
+  </si>
+  <si>
+    <t>ejDAI3dUSVG</t>
+  </si>
+  <si>
+    <t>JkynZtDjpZy</t>
+  </si>
+  <si>
+    <t>ct9VxVIL9Ni</t>
+  </si>
+  <si>
+    <t>t8nUT8zyZYE</t>
+  </si>
+  <si>
+    <t>w6qIJOCUnaB</t>
+  </si>
+  <si>
+    <t>DOozMz365an</t>
+  </si>
+  <si>
+    <t>lCrP5C6yEgR</t>
+  </si>
+  <si>
+    <t>JvnyXYumNDu</t>
+  </si>
+  <si>
+    <t>jitjBxY8hif</t>
+  </si>
+  <si>
+    <t>SQZ8dZYHBLN</t>
+  </si>
+  <si>
+    <t>ic1LXzD8Few</t>
+  </si>
+  <si>
+    <t>SBrrHEwbkKG</t>
+  </si>
+  <si>
+    <t>oFLGt2vGzR5</t>
+  </si>
+  <si>
+    <t>owMNSPY8rtf</t>
+  </si>
+  <si>
+    <t>kbiAIf1nAF2</t>
+  </si>
+  <si>
+    <t>LU37gpCIMjp</t>
+  </si>
+  <si>
+    <t>v1pl5APemJj</t>
+  </si>
+  <si>
+    <t>Xkpfm4eoUOQ</t>
+  </si>
+  <si>
+    <t>rZ9FQN7N359</t>
+  </si>
+  <si>
+    <t>IORrwxfgIaI</t>
+  </si>
+  <si>
+    <t>STShzXdk2pE</t>
+  </si>
+  <si>
+    <t>bWGnr6Ozn69</t>
+  </si>
+  <si>
+    <t>zm52lh7e051</t>
+  </si>
+  <si>
+    <t>FfezJcC8G6g</t>
+  </si>
+  <si>
+    <t>dfHrK7oeMvs</t>
+  </si>
+  <si>
+    <t>K6aIR0qKyEl</t>
+  </si>
+  <si>
+    <t>uW8Zm6u2YXp</t>
+  </si>
+  <si>
+    <t>fHXmHefLKkR</t>
+  </si>
+  <si>
+    <t>XSezAtiYRds</t>
+  </si>
+  <si>
+    <t>Xy1pTfzqULU</t>
+  </si>
+  <si>
+    <t>UZ0hY2Wu6NT</t>
+  </si>
+  <si>
+    <t>QHiujlAKZpX</t>
+  </si>
+  <si>
+    <t>ZWvPaRBLLCd</t>
+  </si>
+  <si>
+    <t>NyIL2imxFxe</t>
+  </si>
+  <si>
+    <t>wwGrpAczt6y</t>
+  </si>
+  <si>
+    <t>VO4BTcjcBV3</t>
+  </si>
+  <si>
+    <t>eob4QOoF7LO</t>
+  </si>
+  <si>
+    <t>iZtXv1Nwop6</t>
+  </si>
+  <si>
+    <t>eo3jLNriZmG</t>
+  </si>
+  <si>
+    <t>Y9aV9Fsh9DZ</t>
+  </si>
+  <si>
+    <t>w2mRPcVCdeD</t>
+  </si>
+  <si>
+    <t>kg8UmJESl05</t>
+  </si>
+  <si>
+    <t>Veq7rVwC3l0</t>
+  </si>
+  <si>
+    <t>ukQmb8aHJ4m</t>
+  </si>
+  <si>
+    <t>ZuIe96dFPBy</t>
+  </si>
+  <si>
+    <t>xRJuSMNCtLN</t>
+  </si>
+  <si>
+    <t>xnKdq6TMFJM</t>
+  </si>
+  <si>
+    <t>mw7pzY4LKBQ</t>
+  </si>
+  <si>
+    <t>Hk9BG20VX8r</t>
+  </si>
+  <si>
+    <t>xoTVrNjcSXB</t>
+  </si>
+  <si>
+    <t>OfkldNGx6rp</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Clients of FSWs age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive FSWs age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSM age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive MSW age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 10-14 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 1-4 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 15-19 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age &lt;1 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 50+yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Female age 5-9 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 10-14 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 1-4 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 15-19 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age &lt;1 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive Other Male age 5-9 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG Non SW age 50+ yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 20-24 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age &lt;20 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 25-29 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 30-34 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 35-39 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 40-44 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 45-49 yrs</t>
+  </si>
+  <si>
+    <t>CLT - HIV Index Screened reactive TG SW age 50+ yrs</t>
   </si>
 </sst>
 </file>
@@ -87,9 +555,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,16 +875,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F668FD1-C67A-4E03-AE66-3FE08B900D4F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -425,19 +896,643 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -446,15 +1541,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -651,6 +1737,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -658,14 +1753,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -684,6 +1771,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>

</xml_diff>